<commit_message>
Update geral de todos os arquivos para as versões mais recentes utilizadas; modificações na estrutura de pastas; add de novos arquivos; remoção e/ou substituição de arquivos defasados; Add da pasta GitHub CLI.
</commit_message>
<xml_diff>
--- a/Excel/exercicios 1.1 1.2 1.3 1.4.xlsx
+++ b/Excel/exercicios 1.1 1.2 1.3 1.4.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="1.1" sheetId="1" state="visible" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Nome</t>
   </si>
@@ -90,13 +90,22 @@
     <t>Pão</t>
   </si>
   <si>
-    <t>Ovos</t>
-  </si>
-  <si>
-    <t>Arroz</t>
-  </si>
-  <si>
-    <t>Frango</t>
+    <t xml:space="preserve">Custo Unitário</t>
+  </si>
+  <si>
+    <t>Lucro</t>
+  </si>
+  <si>
+    <t>Adição</t>
+  </si>
+  <si>
+    <t>Multiplicação</t>
+  </si>
+  <si>
+    <t>Subtração</t>
+  </si>
+  <si>
+    <t>Divisão</t>
   </si>
   <si>
     <t>Boletim</t>
@@ -139,7 +148,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11.000000"/>
       <color theme="1"/>
@@ -160,11 +169,15 @@
     </font>
     <font>
       <sz val="10.000000"/>
-      <color indexed="64"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="11.000000"/>
+      <color indexed="64"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -181,6 +194,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="5"/>
+        <bgColor indexed="5"/>
       </patternFill>
     </fill>
   </fills>
@@ -211,17 +230,17 @@
       <left style="thin">
         <color rgb="FFCCCCCC"/>
       </left>
-      <right/>
+      <right style="none"/>
       <top style="thin">
         <color rgb="FFCCCCCC"/>
       </top>
       <bottom style="thin">
         <color rgb="FFCCCCCC"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none"/>
     </border>
     <border>
-      <left/>
+      <left style="none"/>
       <right style="thin">
         <color rgb="FFCCCCCC"/>
       </right>
@@ -231,7 +250,7 @@
       <bottom style="thin">
         <color rgb="FFCCCCCC"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none"/>
     </border>
   </borders>
   <cellStyleXfs count="3">
@@ -239,7 +258,7 @@
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="2" fillId="3" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="3" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -270,11 +289,20 @@
     </xf>
     <xf fontId="2" fillId="3" borderId="0" numFmtId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf fontId="4" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -860,7 +888,7 @@
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157500000008" bottom="0.78740157500000008" header="0.31496062000000008" footer="0.31496062000000008"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157500000008" bottom="0.78740157500000008" header="0.31496062000000014" footer="0.31496062000000014"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
@@ -973,113 +1001,144 @@
         <v>16</v>
       </c>
       <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
     </row>
     <row r="2">
-      <c r="B2" t="s">
+      <c r="B2" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3">
-      <c r="B3" t="s">
+      <c r="B3" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="15">
         <v>3</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="15">
         <v>2.5</v>
       </c>
+      <c r="E3" s="13"/>
     </row>
     <row r="4">
-      <c r="B4" t="s">
+      <c r="B4" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="15">
         <v>1</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="15">
         <v>4</v>
       </c>
+      <c r="E4" s="13"/>
     </row>
     <row r="5">
-      <c r="B5" t="s">
+      <c r="B5" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="15">
         <v>2</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="15">
         <v>3.25</v>
       </c>
+      <c r="E5" s="13"/>
     </row>
     <row r="6">
-      <c r="B6" t="s">
+      <c r="B6" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+    </row>
+    <row r="7">
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+    </row>
+    <row r="8">
+      <c r="B8" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C6">
-        <v>12</v>
-      </c>
-      <c r="D6">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" t="s">
+      <c r="E8" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" t="s">
+    </row>
+    <row r="9">
+      <c r="B9" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="D9" s="15">
+        <v>1.5</v>
+      </c>
+      <c r="E9" s="13"/>
+    </row>
+    <row r="10">
+      <c r="B10" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="15">
+        <v>4</v>
+      </c>
+      <c r="D10" s="15">
+        <v>2</v>
+      </c>
+      <c r="E10" s="13"/>
+    </row>
+    <row r="11">
+      <c r="B11" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="15">
+        <v>3.25</v>
+      </c>
+      <c r="D11" s="15">
+        <v>2.3500000000000001</v>
+      </c>
+      <c r="E11" s="13"/>
+    </row>
+    <row r="12">
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+    </row>
+    <row r="13" ht="15">
+      <c r="B13" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C8">
-        <v>1.5</v>
-      </c>
-      <c r="D8">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9"/>
-      <c r="C9"/>
-      <c r="D9"/>
-    </row>
-    <row r="10">
-      <c r="B10"/>
-      <c r="C10"/>
-      <c r="D10"/>
-    </row>
-    <row r="11">
-      <c r="B11"/>
-      <c r="C11"/>
-      <c r="D11"/>
-    </row>
-    <row r="12">
-      <c r="B12"/>
-      <c r="C12"/>
-      <c r="D12"/>
+      <c r="C13" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:E1"/>
-  </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
@@ -1102,34 +1161,34 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
+      <c r="B1" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="2">
       <c r="B2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C3">
         <v>8.5</v>
@@ -1143,7 +1202,7 @@
     </row>
     <row r="4">
       <c r="B4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C4">
         <v>7</v>
@@ -1157,7 +1216,7 @@
     </row>
     <row r="5">
       <c r="B5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C5">
         <v>9</v>
@@ -1171,7 +1230,7 @@
     </row>
     <row r="6">
       <c r="B6" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C6">
         <v>6.5</v>
@@ -1185,7 +1244,7 @@
     </row>
     <row r="7">
       <c r="B7" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C7">
         <v>8</v>

</xml_diff>